<commit_message>
Progres + test img
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">Toujours vérifier que les ratio de contraste texte/fond sont conformes aux exigences du WCAG</t>
   </si>
   <si>
-    <t xml:space="preserve">Ajuster les couleurs de ces passages</t>
+    <t xml:space="preserve">Ajuster les contrastes couleurs</t>
   </si>
   <si>
     <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/Accessibility/Understanding_WCAG/Perceivable/Color_contrast</t>
@@ -116,13 +116,13 @@
     <t xml:space="preserve">Trop grand nombre de liens partenaires et annuaires en bas de la page</t>
   </si>
   <si>
-    <t xml:space="preserve">Trop de liens risque d’impacter négativement le SEO et peut même être reconnu comme une tentative de Blackhat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limiter le nombre de liens de la page pour conserver ceux importants au site + définir dans le code ceux que le bot de référencement ne doit pas suivre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diminuer le nombre de liens et définir ceux à ne pas suivre</t>
+    <t xml:space="preserve">Trop de liens sans pertinence par rapport au contenu du site risque d’impacter négativement le SEO et peut même être reconnu comme une tentative de Blackhat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limiter le nombre de liens de la page pour conserver ceux pertinents + définir dans le code ceux que le bot de référencement ne doit pas suivre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vérifier quels liens sont pertinents et supprimer les autres</t>
   </si>
   <si>
     <t xml:space="preserve">https://semji.com/fr/guide/backlink-en-seo/</t>
@@ -155,16 +155,16 @@
     <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Learn/HTML/Introduction_to_HTML/The_head_metadata_in_HTML#d%C3%A9finition_de_la_langue_principale_du_document</t>
   </si>
   <si>
-    <t xml:space="preserve">Liens réseaux sociaux sans texte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les lecteurs d’écran indiqueront la présence de ces liens mais l’utilisateur ne pourra pas connaître leur utilité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toujours rendre clair l’utilité de chaque lien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remplir le texte des liens</t>
+    <t xml:space="preserve">Liens réseaux sociaux icônes sans étiquette + formulaire sans étiquette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les lecteurs d’écran indiqueront la présence de ces liens et formulaires mais l’utilisateur ne pourra pas connaître leur utilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toujours rendre clair l’utilité de chaque élément sans texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer des étiquettes</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.accede-web.com/notices/html-et-css/liens-et-boutons/completer-les-liens-et-les-boutons-non-explicites-avec-aria-label-ou-title/</t>
@@ -266,7 +266,7 @@
     <t xml:space="preserve">La page contact appelle les mauvais fichiers de style</t>
   </si>
   <si>
-    <t xml:space="preserve">Si une page n’appelle pas correctement toutes les fichiers de style dont elle a besoin son affiche en sera forcément très impacté</t>
+    <t xml:space="preserve">Si une page n’appelle pas correctement toutes les fichiers de style dont elle a besoin son affichage en sera forcément très impacté</t>
   </si>
   <si>
     <t xml:space="preserve">Vérifier que tous les fichiers de styles auxquelles les pages font appel sont les bons</t>
@@ -314,16 +314,16 @@
     <t xml:space="preserve">Résoudre les problèmes repérés par le validateur</t>
   </si>
   <si>
-    <t xml:space="preserve">Texte du bandeau de la page Contact illisible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Très peu d’utilisateurs sauront que ce texte est là et il risque d’être considéré comme une tentative de BlackHat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vérifier qu’aucun contenu n’est invisible pour une raison où une autre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changer la couleur du texte du bandeau</t>
+    <t xml:space="preserve">Mauvais format des images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Des images dans des formats inadaptés peuvent ralentir le chargement de la page ce qui impacte le référencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enregistrer les images utilisées dans des formats adaptés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convertir les images</t>
   </si>
   <si>
     <t xml:space="preserve">Action réalisée</t>
@@ -332,10 +332,10 @@
     <t xml:space="preserve">OUI</t>
   </si>
   <si>
+    <t xml:space="preserve">Pas Certain</t>
+  </si>
+  <si>
     <t xml:space="preserve">NON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commencé</t>
   </si>
 </sst>
 </file>
@@ -442,14 +442,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8D281E"/>
-        <bgColor rgb="FF993366"/>
+        <fgColor rgb="FF2A6099"/>
+        <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6B5E9B"/>
-        <bgColor rgb="FF808080"/>
+        <fgColor rgb="FF8D281E"/>
+        <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
   </fills>
@@ -576,7 +576,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -600,7 +600,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF6B5E9B"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -622,11 +622,11 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.51"/>
@@ -1028,12 +1028,22 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+    <row r="20" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1060,22 +1070,12 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>100</v>
-      </c>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2219,13 +2219,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.69921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.2"/>
   </cols>
@@ -2266,16 +2266,16 @@
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>103</v>
+      <c r="B5" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>103</v>
+      <c r="B6" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,24 +2314,24 @@
       <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>103</v>
+      <c r="B11" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>104</v>
+      <c r="B12" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>103</v>
+      <c r="B13" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,15 +2344,15 @@
     </row>
     <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>103</v>
+        <v>87</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>102</v>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>102</v>
@@ -2368,30 +2368,27 @@
     </row>
     <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
+      <c r="B20" s="11" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
@@ -2406,7 +2403,7 @@
       <c r="A26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4"/>
+      <c r="A27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
@@ -2424,7 +2421,7 @@
       <c r="A32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8"/>
+      <c r="A33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7"/>
@@ -2453,9 +2450,7 @@
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>